<commit_message>
Da's edits to a pretty cool program
</commit_message>
<xml_diff>
--- a/prices.xlsx
+++ b/prices.xlsx
@@ -31,7 +31,7 @@
     <t>iPhone 6, 64 GB, unlocked</t>
   </si>
   <si>
-    <t>$103</t>
+    <t>$102</t>
   </si>
   <si>
     <t>iPhone 6, 128 GB, unlocked</t>
@@ -103,7 +103,7 @@
     <t>iPhone 6 Plus, 64 GB, unlocked</t>
   </si>
   <si>
-    <t>$141</t>
+    <t>$140</t>
   </si>
   <si>
     <t>iPhone 6 Plus, 128 GB, unlocked</t>
@@ -247,13 +247,13 @@
     <t>iPhone 6S Plus, 64 GB, unlocked</t>
   </si>
   <si>
-    <t>$178</t>
+    <t>$179</t>
   </si>
   <si>
     <t>iPhone 6S Plus, 128 GB, unlocked</t>
   </si>
   <si>
-    <t>$191</t>
+    <t>$192</t>
   </si>
   <si>
     <t>iPhone 6S Plus, 16 GB, verizon</t>
@@ -313,7 +313,7 @@
     <t>iPhone 7, 128 GB, unlocked</t>
   </si>
   <si>
-    <t>$186</t>
+    <t>$187</t>
   </si>
   <si>
     <t>iPhone 7, 256 GB, unlocked</t>
@@ -373,7 +373,7 @@
     <t>iPhone 7 Plus, 256 GB, unlocked</t>
   </si>
   <si>
-    <t>$282</t>
+    <t>$281</t>
   </si>
   <si>
     <t>iPhone 7 Plus, 32 GB, verizon</t>
@@ -427,7 +427,7 @@
     <t>iPhone 8, 256 GB, unlocked</t>
   </si>
   <si>
-    <t>$311</t>
+    <t>$312</t>
   </si>
   <si>
     <t>iPhone 8, 64 GB, verizon</t>
@@ -469,7 +469,7 @@
     <t>iPhone 8 Plus, 64 GB, unlocked</t>
   </si>
   <si>
-    <t>$337</t>
+    <t>$336</t>
   </si>
   <si>
     <t>iPhone 8 Plus, 128 GB, unlocked</t>
@@ -481,7 +481,7 @@
     <t>iPhone 8 Plus, 256 GB, unlocked</t>
   </si>
   <si>
-    <t>$388</t>
+    <t>$389</t>
   </si>
   <si>
     <t>iPhone 8 Plus, 64 GB, verizon</t>
@@ -523,7 +523,7 @@
     <t>iPhone X, 64 GB, unlocked</t>
   </si>
   <si>
-    <t>$409</t>
+    <t>$408</t>
   </si>
   <si>
     <t>iPhone X, 256 GB, unlocked</t>
@@ -559,7 +559,7 @@
     <t>iPhone Xr, 64 GB, unlocked</t>
   </si>
   <si>
-    <t>$420</t>
+    <t>$419</t>
   </si>
   <si>
     <t>iPhone Xr, 128 GB, unlocked</t>
@@ -616,57 +616,57 @@
     <t>iPhone Xs, 256 GB, unlocked</t>
   </si>
   <si>
+    <t>$540</t>
+  </si>
+  <si>
+    <t>iPhone Xs, 512 GB, unlocked</t>
+  </si>
+  <si>
+    <t>$560</t>
+  </si>
+  <si>
+    <t>iPhone Xs, 64 GB, verizon</t>
+  </si>
+  <si>
+    <t>iPhone Xs, 256 GB, verizon</t>
+  </si>
+  <si>
+    <t>iPhone Xs, 512 GB, verizon</t>
+  </si>
+  <si>
+    <t>iPhone Xs, 64 GB, att</t>
+  </si>
+  <si>
+    <t>iPhone Xs, 256 GB, att</t>
+  </si>
+  <si>
+    <t>iPhone Xs, 512 GB, att</t>
+  </si>
+  <si>
+    <t>iPhone Xs, 64 GB, t-mobile</t>
+  </si>
+  <si>
+    <t>iPhone Xs, 256 GB, t-mobile</t>
+  </si>
+  <si>
+    <t>iPhone Xs, 512 GB, t-mobile</t>
+  </si>
+  <si>
+    <t>iPhone Xs, 64 GB, sprint</t>
+  </si>
+  <si>
+    <t>iPhone Xs, 256 GB, sprint</t>
+  </si>
+  <si>
+    <t>iPhone Xs, 512 GB, sprint</t>
+  </si>
+  <si>
+    <t>iPhone Xs Max, 64 GB, unlocked</t>
+  </si>
+  <si>
     <t>$542</t>
   </si>
   <si>
-    <t>iPhone Xs, 512 GB, unlocked</t>
-  </si>
-  <si>
-    <t>$560</t>
-  </si>
-  <si>
-    <t>iPhone Xs, 64 GB, verizon</t>
-  </si>
-  <si>
-    <t>iPhone Xs, 256 GB, verizon</t>
-  </si>
-  <si>
-    <t>iPhone Xs, 512 GB, verizon</t>
-  </si>
-  <si>
-    <t>iPhone Xs, 64 GB, att</t>
-  </si>
-  <si>
-    <t>iPhone Xs, 256 GB, att</t>
-  </si>
-  <si>
-    <t>iPhone Xs, 512 GB, att</t>
-  </si>
-  <si>
-    <t>iPhone Xs, 64 GB, t-mobile</t>
-  </si>
-  <si>
-    <t>iPhone Xs, 256 GB, t-mobile</t>
-  </si>
-  <si>
-    <t>iPhone Xs, 512 GB, t-mobile</t>
-  </si>
-  <si>
-    <t>iPhone Xs, 64 GB, sprint</t>
-  </si>
-  <si>
-    <t>iPhone Xs, 256 GB, sprint</t>
-  </si>
-  <si>
-    <t>iPhone Xs, 512 GB, sprint</t>
-  </si>
-  <si>
-    <t>iPhone Xs Max, 64 GB, unlocked</t>
-  </si>
-  <si>
-    <t>$543</t>
-  </si>
-  <si>
     <t>iPhone Xs Max, 256 GB, unlocked</t>
   </si>
   <si>
@@ -718,7 +718,7 @@
     <t>iPhone 11, 64 GB, unlocked</t>
   </si>
   <si>
-    <t>$608</t>
+    <t>$607</t>
   </si>
   <si>
     <t>iPhone 11, 128 GB, unlocked</t>
@@ -772,19 +772,19 @@
     <t>iPhone 11 Pro, 64 GB, unlocked</t>
   </si>
   <si>
-    <t>$774</t>
+    <t>$773</t>
   </si>
   <si>
     <t>iPhone 11 Pro, 256 GB, unlocked</t>
   </si>
   <si>
-    <t>$885</t>
+    <t>$884</t>
   </si>
   <si>
     <t>iPhone 11 Pro, 512 GB, unlocked</t>
   </si>
   <si>
-    <t>$965</t>
+    <t>$962</t>
   </si>
   <si>
     <t>iPhone 11 Pro, 64 GB, verizon</t>
@@ -826,19 +826,19 @@
     <t>iPhone 11 Pro Max, 64 GB, unlocked</t>
   </si>
   <si>
-    <t>$861</t>
+    <t>$860</t>
   </si>
   <si>
     <t>iPhone 11 Pro Max, 256 GB, unlocked</t>
   </si>
   <si>
-    <t>$949</t>
+    <t>$948</t>
   </si>
   <si>
     <t>iPhone 11 Pro Max, 512 GB, unlocked</t>
   </si>
   <si>
-    <t>$1053</t>
+    <t>$1050</t>
   </si>
   <si>
     <t>iPhone 11 Pro Max, 64 GB, verizon</t>
@@ -880,7 +880,7 @@
     <t>iPhone SE 2nd Gen, 64 GB, unlocked</t>
   </si>
   <si>
-    <t>$344</t>
+    <t>$343</t>
   </si>
   <si>
     <t>iPhone SE 2nd Gen, 128 GB, unlocked</t>

</xml_diff>